<commit_message>
Added runnable integration without main clock
</commit_message>
<xml_diff>
--- a/debug/DebugDataTransfer.xlsx
+++ b/debug/DebugDataTransfer.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t xml:space="preserve">Instruction (1 Byte)</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Data (2 Byte)</t>
   </si>
   <si>
+    <t xml:space="preserve">Data (2Byte)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Description</t>
   </si>
   <si>
@@ -43,6 +46,9 @@
     <t xml:space="preserve">RegAddr</t>
   </si>
   <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
     <t xml:space="preserve">Get Data From Reg</t>
   </si>
   <si>
@@ -56,6 +62,24 @@
   </si>
   <si>
     <t xml:space="preserve">Data of requested Reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRAM Write</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRAM Write</t>
   </si>
 </sst>
 </file>
@@ -153,22 +177,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="25.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -181,46 +207,80 @@
       <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="0" t="s">
         <v>3</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="H2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Added all mandetory debug functionallity + tests of FPGA
</commit_message>
<xml_diff>
--- a/debug/DebugDataTransfer.xlsx
+++ b/debug/DebugDataTransfer.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="94">
   <si>
     <t xml:space="preserve">Host → FPGA</t>
   </si>
@@ -181,13 +181,28 @@
     <t xml:space="preserve">0x32</t>
   </si>
   <si>
-    <t xml:space="preserve">read_iram</t>
+    <t xml:space="preserve">BankID 4 Bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">read_ram</t>
   </si>
   <si>
     <t xml:space="preserve">data 16bit</t>
   </si>
   <si>
     <t xml:space="preserve">addr 16bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VRAM Write</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMIO Write</t>
   </si>
   <si>
     <t xml:space="preserve">Alu</t>
@@ -386,17 +401,17 @@
   </sheetPr>
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H52" activeCellId="0" sqref="H52"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.71"/>
@@ -700,34 +715,71 @@
       <c r="B52" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="C52" s="0" t="s">
+        <v>53</v>
+      </c>
       <c r="D52" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G52" s="0" t="s">
         <v>52</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="H66" s="0" t="s">
         <v>23</v>
@@ -735,13 +787,13 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="H67" s="0" t="s">
         <v>23</v>
@@ -749,13 +801,13 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="H68" s="0" t="s">
         <v>23</v>
@@ -763,13 +815,13 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H69" s="0" t="s">
         <v>23</v>
@@ -777,13 +829,13 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="H70" s="0" t="s">
         <v>23</v>
@@ -791,58 +843,58 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H84" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="H85" s="0" t="s">
         <v>17</v>
@@ -850,13 +902,13 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="H86" s="0" t="s">
         <v>17</v>
@@ -864,13 +916,13 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H87" s="0" t="s">
         <v>23</v>
@@ -878,13 +930,13 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H88" s="0" t="s">
         <v>23</v>
@@ -892,13 +944,13 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="H89" s="0" t="s">
         <v>23</v>
@@ -906,13 +958,13 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="H90" s="0" t="s">
         <v>23</v>
@@ -920,16 +972,16 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added pipeline_jmp and error tx on wrong instruction request to FPGA
</commit_message>
<xml_diff>
--- a/debug/DebugDataTransfer.xlsx
+++ b/debug/DebugDataTransfer.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="97">
   <si>
     <t xml:space="preserve">Host → FPGA</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t xml:space="preserve">resume clk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 Bit instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instruction Error</t>
   </si>
   <si>
     <t xml:space="preserve">Pipeline</t>
@@ -402,7 +411,7 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -487,501 +496,512 @@
         <v>12</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E50" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G50" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="G50" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="D51" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="H84" s="0" t="s">
         <v>78</v>
-      </c>
-      <c r="E84" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="G84" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H84" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H85" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H86" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H87" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H88" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H89" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed unused signal requests and revomed clock resume load clk checking
</commit_message>
<xml_diff>
--- a/debug/DebugDataTransfer.xlsx
+++ b/debug/DebugDataTransfer.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="93">
   <si>
     <t xml:space="preserve">Host → FPGA</t>
   </si>
@@ -115,12 +115,6 @@
     <t xml:space="preserve">pipeline_operand_2</t>
   </si>
   <si>
-    <t xml:space="preserve">0x15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pipeline_memory_addr_reg</t>
-  </si>
-  <si>
     <t xml:space="preserve">0x16</t>
   </si>
   <si>
@@ -299,12 +293,6 @@
   </si>
   <si>
     <t xml:space="preserve">regfile_reg2_data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">regfile_regma_data</t>
   </si>
   <si>
     <t xml:space="preserve">0x59</t>
@@ -410,8 +398,8 @@
   </sheetPr>
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -595,211 +583,196 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="J24" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>38</v>
-      </c>
       <c r="G34" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H34" s="0" t="s">
         <v>26</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H35" s="0" t="s">
         <v>26</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H36" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="I36" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="G36" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="H36" s="0" t="s">
+      <c r="J36" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="J36" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="10.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="D50" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="E50" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="G50" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D51" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G51" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="E51" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="G51" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E52" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="G52" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H52" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D52" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="E52" s="0" t="s">
+      <c r="I52" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="G52" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="H52" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="I52" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E66" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E66" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="G66" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H66" s="0" t="s">
         <v>26</v>
@@ -807,13 +780,13 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H67" s="0" t="s">
         <v>26</v>
@@ -821,13 +794,13 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H68" s="0" t="s">
         <v>26</v>
@@ -835,13 +808,13 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H69" s="0" t="s">
         <v>26</v>
@@ -849,13 +822,13 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H70" s="0" t="s">
         <v>26</v>
@@ -863,58 +836,58 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E82" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B82" s="0" t="s">
+      <c r="G82" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="H82" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="E82" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="G82" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="H82" s="0" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H84" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G85" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H85" s="0" t="s">
         <v>20</v>
@@ -922,13 +895,13 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H86" s="0" t="s">
         <v>20</v>
@@ -936,13 +909,13 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H87" s="0" t="s">
         <v>26</v>
@@ -950,13 +923,13 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H88" s="0" t="s">
         <v>26</v>
@@ -964,44 +937,31 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H89" s="0" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="E90" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="G90" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="H90" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="0" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new signal read and baudrate to 9600
</commit_message>
<xml_diff>
--- a/debug/DebugDataTransfer.xlsx
+++ b/debug/DebugDataTransfer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\SixteenShadesOfCpu\debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03DDA56-D1C1-4A9F-ACE6-0DB351D6F4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F023C9-EB01-45B3-8793-A4A89C0A85B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7425" yWindow="-16200" windowWidth="14610" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="121">
   <si>
     <t>Host → FPGA</t>
   </si>
@@ -123,9 +123,6 @@
     <t>0x16</t>
   </si>
   <si>
-    <t>pipeline_jmp</t>
-  </si>
-  <si>
     <t>1Bit</t>
   </si>
   <si>
@@ -340,6 +337,57 @@
   </si>
   <si>
     <t>vram read</t>
+  </si>
+  <si>
+    <t>0x18</t>
+  </si>
+  <si>
+    <t>pipeline_immediate_out</t>
+  </si>
+  <si>
+    <t>0x19</t>
+  </si>
+  <si>
+    <t>pipeline_write_address_out</t>
+  </si>
+  <si>
+    <t>0x1A</t>
+  </si>
+  <si>
+    <t>pipeline_whb_wlb_out</t>
+  </si>
+  <si>
+    <t>2 Bit</t>
+  </si>
+  <si>
+    <t>0x1B</t>
+  </si>
+  <si>
+    <t>pipeline_write_data_sel_out</t>
+  </si>
+  <si>
+    <t>0x1C</t>
+  </si>
+  <si>
+    <t>3 Bit</t>
+  </si>
+  <si>
+    <t>0x1D</t>
+  </si>
+  <si>
+    <t>pipeline_RAM_src_read_write_bankid_out</t>
+  </si>
+  <si>
+    <t>7 Bit</t>
+  </si>
+  <si>
+    <t>pipeline_jmp_condl_rel_dests_cond_out</t>
+  </si>
+  <si>
+    <t>7Bit</t>
+  </si>
+  <si>
+    <t>pipeline_is_alu_ram_gpu_op_out</t>
   </si>
 </sst>
 </file>
@@ -713,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="E41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,19 +948,19 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" t="s">
         <v>91</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
+        <v>90</v>
+      </c>
+      <c r="H23" t="s">
         <v>92</v>
       </c>
-      <c r="G23" t="s">
+      <c r="J23" t="s">
         <v>91</v>
-      </c>
-      <c r="H23" t="s">
-        <v>93</v>
-      </c>
-      <c r="J23" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -920,281 +968,383 @@
         <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>118</v>
       </c>
       <c r="G24" t="s">
         <v>31</v>
       </c>
       <c r="H24" t="s">
-        <v>33</v>
+        <v>119</v>
       </c>
       <c r="J24" t="s">
-        <v>32</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" t="s">
         <v>94</v>
       </c>
-      <c r="E25" t="s">
-        <v>95</v>
-      </c>
       <c r="G25" t="s">
+        <v>93</v>
+      </c>
+      <c r="H25" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" t="s">
         <v>94</v>
       </c>
-      <c r="H25" t="s">
-        <v>33</v>
-      </c>
-      <c r="J25" t="s">
-        <v>95</v>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" t="s">
+        <v>107</v>
+      </c>
+      <c r="G27" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27" t="s">
+        <v>73</v>
+      </c>
+      <c r="J27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" t="s">
+        <v>109</v>
+      </c>
+      <c r="G28" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" t="s">
+        <v>110</v>
+      </c>
+      <c r="J28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" t="s">
+        <v>112</v>
+      </c>
+      <c r="G29" t="s">
+        <v>111</v>
+      </c>
+      <c r="H29" t="s">
+        <v>110</v>
+      </c>
+      <c r="J29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>113</v>
+      </c>
+      <c r="E30" t="s">
+        <v>116</v>
+      </c>
+      <c r="G30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H30" t="s">
+        <v>117</v>
+      </c>
+      <c r="J30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" t="s">
+        <v>120</v>
+      </c>
+      <c r="G31" t="s">
+        <v>115</v>
+      </c>
+      <c r="H31" t="s">
+        <v>114</v>
+      </c>
+      <c r="J31" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>34</v>
       </c>
-      <c r="B34" t="s">
+      <c r="E34" t="s">
         <v>35</v>
       </c>
-      <c r="E34" t="s">
-        <v>36</v>
-      </c>
       <c r="G34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H34" t="s">
         <v>26</v>
       </c>
       <c r="J34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" t="s">
         <v>37</v>
       </c>
-      <c r="E35" t="s">
-        <v>38</v>
-      </c>
       <c r="G35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H35" t="s">
         <v>26</v>
       </c>
       <c r="J35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" t="s">
         <v>39</v>
       </c>
-      <c r="E36" t="s">
+      <c r="G36" t="s">
+        <v>38</v>
+      </c>
+      <c r="H36" t="s">
         <v>40</v>
       </c>
-      <c r="G36" t="s">
-        <v>39</v>
-      </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>41</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>42</v>
-      </c>
-      <c r="J36" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" t="s">
         <v>44</v>
-      </c>
-      <c r="E37" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
         <v>46</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>47</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>48</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>49</v>
       </c>
-      <c r="E50" t="s">
-        <v>50</v>
-      </c>
       <c r="G50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" t="s">
+        <v>48</v>
+      </c>
+      <c r="E51" t="s">
         <v>51</v>
       </c>
-      <c r="C51" t="s">
-        <v>48</v>
-      </c>
-      <c r="D51" t="s">
-        <v>49</v>
-      </c>
-      <c r="E51" t="s">
-        <v>52</v>
-      </c>
       <c r="G51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52" t="s">
+        <v>47</v>
+      </c>
+      <c r="E52" t="s">
+        <v>100</v>
+      </c>
+      <c r="G52" t="s">
+        <v>52</v>
+      </c>
+      <c r="H52" t="s">
         <v>53</v>
       </c>
-      <c r="D52" t="s">
-        <v>48</v>
-      </c>
-      <c r="E52" t="s">
-        <v>101</v>
-      </c>
-      <c r="G52" t="s">
-        <v>53</v>
-      </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
         <v>54</v>
-      </c>
-      <c r="I52" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" t="s">
+        <v>48</v>
+      </c>
+      <c r="E53" t="s">
         <v>56</v>
       </c>
-      <c r="C53" t="s">
-        <v>48</v>
-      </c>
-      <c r="D53" t="s">
-        <v>49</v>
-      </c>
-      <c r="E53" t="s">
-        <v>57</v>
-      </c>
       <c r="G53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" t="s">
+        <v>48</v>
+      </c>
+      <c r="E54" t="s">
         <v>58</v>
       </c>
-      <c r="C54" t="s">
-        <v>48</v>
-      </c>
-      <c r="D54" t="s">
-        <v>49</v>
-      </c>
-      <c r="E54" t="s">
-        <v>59</v>
-      </c>
       <c r="G54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G55" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H55" t="s">
+        <v>53</v>
+      </c>
+      <c r="I55" t="s">
         <v>54</v>
-      </c>
-      <c r="I55" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H56" t="s">
+        <v>53</v>
+      </c>
+      <c r="I56" t="s">
         <v>54</v>
-      </c>
-      <c r="I56" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D57" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H57" t="s">
+        <v>53</v>
+      </c>
+      <c r="I57" t="s">
         <v>54</v>
-      </c>
-      <c r="I57" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E58" t="s">
         <v>96</v>
       </c>
-      <c r="E58" t="s">
-        <v>97</v>
-      </c>
       <c r="G58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H58" t="s">
         <v>26</v>
       </c>
       <c r="J58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66" t="s">
         <v>60</v>
       </c>
-      <c r="B66" t="s">
+      <c r="E66" t="s">
         <v>61</v>
       </c>
-      <c r="E66" t="s">
-        <v>62</v>
-      </c>
       <c r="G66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H66" t="s">
         <v>26</v>
@@ -1202,13 +1352,13 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
+        <v>62</v>
+      </c>
+      <c r="E67" t="s">
         <v>63</v>
       </c>
-      <c r="E67" t="s">
-        <v>64</v>
-      </c>
       <c r="G67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H67" t="s">
         <v>26</v>
@@ -1216,13 +1366,13 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
+        <v>64</v>
+      </c>
+      <c r="E68" t="s">
         <v>65</v>
       </c>
-      <c r="E68" t="s">
-        <v>66</v>
-      </c>
       <c r="G68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H68" t="s">
         <v>26</v>
@@ -1230,13 +1380,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
+        <v>66</v>
+      </c>
+      <c r="E69" t="s">
         <v>67</v>
       </c>
-      <c r="E69" t="s">
-        <v>68</v>
-      </c>
       <c r="G69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H69" t="s">
         <v>26</v>
@@ -1244,13 +1394,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
+        <v>68</v>
+      </c>
+      <c r="E70" t="s">
         <v>69</v>
       </c>
-      <c r="E70" t="s">
-        <v>70</v>
-      </c>
       <c r="G70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H70" t="s">
         <v>26</v>
@@ -1258,58 +1408,58 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>70</v>
+      </c>
+      <c r="B82" t="s">
         <v>71</v>
       </c>
-      <c r="B82" t="s">
+      <c r="E82" t="s">
         <v>72</v>
       </c>
-      <c r="E82" t="s">
+      <c r="G82" t="s">
+        <v>71</v>
+      </c>
+      <c r="H82" t="s">
         <v>73</v>
-      </c>
-      <c r="G82" t="s">
-        <v>72</v>
-      </c>
-      <c r="H82" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
+        <v>74</v>
+      </c>
+      <c r="E83" t="s">
         <v>75</v>
       </c>
-      <c r="E83" t="s">
-        <v>76</v>
-      </c>
       <c r="G83" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H83" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
+        <v>76</v>
+      </c>
+      <c r="E84" t="s">
         <v>77</v>
       </c>
-      <c r="E84" t="s">
-        <v>78</v>
-      </c>
       <c r="G84" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H84" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
+        <v>78</v>
+      </c>
+      <c r="E85" t="s">
         <v>79</v>
       </c>
-      <c r="E85" t="s">
-        <v>80</v>
-      </c>
       <c r="G85" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H85" t="s">
         <v>20</v>
@@ -1317,13 +1467,13 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
+        <v>80</v>
+      </c>
+      <c r="E86" t="s">
         <v>81</v>
       </c>
-      <c r="E86" t="s">
-        <v>82</v>
-      </c>
       <c r="G86" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H86" t="s">
         <v>20</v>
@@ -1331,13 +1481,13 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
+        <v>82</v>
+      </c>
+      <c r="E87" t="s">
         <v>83</v>
       </c>
-      <c r="E87" t="s">
-        <v>84</v>
-      </c>
       <c r="G87" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H87" t="s">
         <v>26</v>
@@ -1345,13 +1495,13 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
+        <v>84</v>
+      </c>
+      <c r="E88" t="s">
         <v>85</v>
       </c>
-      <c r="E88" t="s">
-        <v>86</v>
-      </c>
       <c r="G88" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H88" t="s">
         <v>26</v>
@@ -1359,13 +1509,13 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
+        <v>86</v>
+      </c>
+      <c r="E89" t="s">
         <v>87</v>
       </c>
-      <c r="E89" t="s">
-        <v>88</v>
-      </c>
       <c r="G89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H89" t="s">
         <v>26</v>
@@ -1373,16 +1523,16 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
+        <v>88</v>
+      </c>
+      <c r="E91" t="s">
         <v>89</v>
       </c>
-      <c r="E91" t="s">
-        <v>90</v>
-      </c>
       <c r="G91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H91" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ack for debugger
</commit_message>
<xml_diff>
--- a/debug/DebugDataTransfer.xlsx
+++ b/debug/DebugDataTransfer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\SixteenShadesOfCpu\debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C91FF14-22BF-469C-966C-B93216C17474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69365E96-BDBD-4E37-821E-4FA14EF39868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="123">
   <si>
     <t>Host → FPGA</t>
   </si>
@@ -147,9 +147,27 @@
     <t>1Bit</t>
   </si>
   <si>
+    <t>0x18</t>
+  </si>
+  <si>
+    <t>pipeline_immediate_out</t>
+  </si>
+  <si>
+    <t>0x19</t>
+  </si>
+  <si>
+    <t>pipeline_write_address_out</t>
+  </si>
+  <si>
     <t>4 Bit</t>
   </si>
   <si>
+    <t>0x1A</t>
+  </si>
+  <si>
+    <t>pipeline_whb_wlb_out</t>
+  </si>
+  <si>
     <t>2 Bit</t>
   </si>
   <si>
@@ -166,6 +184,15 @@
   </si>
   <si>
     <t>7 Bit</t>
+  </si>
+  <si>
+    <t>0x1D</t>
+  </si>
+  <si>
+    <t>pipeline_is_alu_ram_gpu_op_out</t>
+  </si>
+  <si>
+    <t>3 Bit</t>
   </si>
   <si>
     <t>Divers signal request</t>
@@ -740,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,10 +855,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="E16" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -984,286 +1011,354 @@
         <v>38</v>
       </c>
     </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" t="s">
+        <v>44</v>
+      </c>
+      <c r="J27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="G29" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H29" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="J29" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E30" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G30" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="H30" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J30" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" t="s">
+        <v>54</v>
+      </c>
+      <c r="G31" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" t="s">
+        <v>55</v>
+      </c>
+      <c r="J31" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E34" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="G34" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="H34" t="s">
         <v>26</v>
       </c>
       <c r="J34" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E35" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="G35" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="H35" t="s">
         <v>26</v>
       </c>
       <c r="J35" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E36" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="G36" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="H36" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="I36" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="J36" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E37" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B50" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D50" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E50" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="G50" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D51" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E51" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="G51" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D52" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="E52" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="G52" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="H52" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="I52" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" t="s">
         <v>70</v>
       </c>
-      <c r="C53" t="s">
-        <v>61</v>
-      </c>
       <c r="D53" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E53" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="G53" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C54" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D54" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E54" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="G54" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D55" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="E55" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G55" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="H55" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="I55" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D56" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="E56" t="s">
+        <v>86</v>
+      </c>
+      <c r="G56" t="s">
+        <v>85</v>
+      </c>
+      <c r="H56" t="s">
         <v>77</v>
       </c>
-      <c r="G56" t="s">
-        <v>76</v>
-      </c>
-      <c r="H56" t="s">
-        <v>68</v>
-      </c>
       <c r="I56" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
+        <v>87</v>
+      </c>
+      <c r="D57" t="s">
+        <v>70</v>
+      </c>
+      <c r="E57" t="s">
+        <v>88</v>
+      </c>
+      <c r="G57" t="s">
+        <v>87</v>
+      </c>
+      <c r="H57" t="s">
+        <v>77</v>
+      </c>
+      <c r="I57" t="s">
         <v>78</v>
-      </c>
-      <c r="D57" t="s">
-        <v>61</v>
-      </c>
-      <c r="E57" t="s">
-        <v>79</v>
-      </c>
-      <c r="G57" t="s">
-        <v>78</v>
-      </c>
-      <c r="H57" t="s">
-        <v>68</v>
-      </c>
-      <c r="I57" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E58" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="G58" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="H58" t="s">
         <v>26</v>
       </c>
       <c r="J58" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E66" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="G66" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="H66" t="s">
         <v>26</v>
@@ -1271,13 +1366,13 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="E67" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="G67" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="H67" t="s">
         <v>26</v>
@@ -1285,13 +1380,13 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="E68" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="G68" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="H68" t="s">
         <v>26</v>
@@ -1299,13 +1394,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="E69" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="G69" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H69" t="s">
         <v>26</v>
@@ -1313,13 +1408,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="E70" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="G70" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="H70" t="s">
         <v>26</v>
@@ -1327,58 +1422,58 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B82" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="E82" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="G82" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="H82" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="E83" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="G83" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="H83" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="E84" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="G84" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="H84" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="E85" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="G85" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="H85" t="s">
         <v>20</v>
@@ -1386,13 +1481,13 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="E86" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="G86" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="H86" t="s">
         <v>20</v>
@@ -1400,13 +1495,13 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="E87" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G87" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="H87" t="s">
         <v>26</v>
@@ -1414,13 +1509,13 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="E88" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="G88" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="H88" t="s">
         <v>26</v>
@@ -1428,13 +1523,13 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="E89" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="G89" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="H89" t="s">
         <v>26</v>
@@ -1442,16 +1537,16 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="E91" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="G91" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="H91" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>